<commit_message>
R script to filter to only outdoor sensors that were active in 2022. The corresponding excel file has been updated.
</commit_message>
<xml_diff>
--- a/data/working_sensor_ids.xlsx
+++ b/data/working_sensor_ids.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Purple Air Research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6985D94D-A468-3246-ABC5-750EE06FD6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BF7503-FD60-3A4F-BF42-60AF8705930B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13960" yWindow="740" windowWidth="15440" windowHeight="16920" xr2:uid="{B76F21CA-0ADE-4F2D-872A-FD7B585C1C39}"/>
+    <workbookView xWindow="6260" yWindow="740" windowWidth="23140" windowHeight="16880" xr2:uid="{B76F21CA-0ADE-4F2D-872A-FD7B585C1C39}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,13 +77,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -390,275 +405,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE9394-B2C2-4E39-944B-445B165DB149}">
-  <dimension ref="A1:A52"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>148545</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>113959</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>4404</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>51933</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>101643</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4395</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>43955</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>151082</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>150042</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>124737</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>124685</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>57579</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>137622</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>124737</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>124677</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>96933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>52011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>56135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>87741</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>3499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>109598</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>5588</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>101643</v>
+      <c r="A17" s="1">
+        <v>8476</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>140390</v>
+      <c r="A18" s="1">
+        <v>7920</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>124513</v>
+      <c r="A19" s="1">
+        <v>113494</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>148029</v>
+      <c r="A20" s="1">
+        <v>5774</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>96933</v>
+      <c r="A21" s="1">
+        <v>96035</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>52011</v>
+      <c r="A22" s="1">
+        <v>94003</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>56135</v>
+      <c r="A23" s="1">
+        <v>140102</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>87741</v>
+      <c r="A24" s="1">
+        <v>96079</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>3499</v>
+      <c r="A25" s="1">
+        <v>39173</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>109598</v>
+      <c r="A26" s="1">
+        <v>124679</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>151188</v>
+      <c r="A27" s="1">
+        <v>128349</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>36901</v>
+      <c r="A28" s="1">
+        <v>124649</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>5588</v>
+      <c r="A29" s="1">
+        <v>77067</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>133664</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>8476</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>6546</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>7920</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>113494</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>5774</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>96035</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>94003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>140102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>96079</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39173</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>124679</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>155131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>128349</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>124649</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>148545</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>4404</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>45079</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>39173</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>57645</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>77067</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>128439</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A30" s="1">
         <v>107560</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A31:A46">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
November data and corresponding working ids.
</commit_message>
<xml_diff>
--- a/data/working_sensor_ids.xlsx
+++ b/data/working_sensor_ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Purple Air Research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BF7503-FD60-3A4F-BF42-60AF8705930B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD9CC2A-F2AD-8141-8588-0578827F2235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="740" windowWidth="23140" windowHeight="16880" xr2:uid="{B76F21CA-0ADE-4F2D-872A-FD7B585C1C39}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,9 +77,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,167 +404,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE9394-B2C2-4E39-944B-445B165DB149}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>113959</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>4404</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>51933</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>101643</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>4395</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>124737</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>124685</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>124677</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>96933</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>52011</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>56135</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>87741</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>3499</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>109598</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>5588</v>
       </c>
     </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>8476</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>8476</v>
+      <c r="A17">
+        <v>7920</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>7920</v>
+      <c r="A18">
+        <v>113494</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>113494</v>
+      <c r="A19">
+        <v>5774</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>5774</v>
+      <c r="A20">
+        <v>96035</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>96035</v>
+      <c r="A21">
+        <v>94003</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>94003</v>
+      <c r="A22">
+        <v>140102</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>140102</v>
+      <c r="A23">
+        <v>96079</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>96079</v>
+      <c r="A24">
+        <v>39173</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>39173</v>
+      <c r="A25">
+        <v>124679</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>124679</v>
+      <c r="A26">
+        <v>124649</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>128349</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>124649</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>77067</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
+      <c r="A27">
         <v>107560</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A31:A46">
+  <conditionalFormatting sqref="A28:A43">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
January data, working sensor ids is now all outdoor sensors active for 2022.
</commit_message>
<xml_diff>
--- a/data/working_sensor_ids.xlsx
+++ b/data/working_sensor_ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/personal/Purple Air Research/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD9CC2A-F2AD-8141-8588-0578827F2235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D4CFB9-8E2F-AA49-B1BF-EC2F9045E15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="740" windowWidth="23140" windowHeight="16880" xr2:uid="{B76F21CA-0ADE-4F2D-872A-FD7B585C1C39}"/>
   </bookViews>
@@ -77,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,152 +405,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DE9394-B2C2-4E39-944B-445B165DB149}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>113959</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>4404</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>51933</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>101643</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4395</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>124737</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>124685</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>124737</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>124677</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>101643</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>96933</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>52011</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>56135</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>87741</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>3499</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>109598</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>5588</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>8476</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>41581</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>7920</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>113494</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
         <v>5774</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>96035</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
         <v>94003</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
         <v>140102</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>96079</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>39173</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>124679</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>128349</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>124649</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>4404</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>39173</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>77067</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>120369</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>107560</v>
       </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A28:A43">
-    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
+  <conditionalFormatting sqref="A39:A43">
+    <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>